<commit_message>
[Minno, Juan] #203 fixed tests for import students
</commit_message>
<xml_diff>
--- a/tools/import-student-records/test/Test.xlsx
+++ b/tools/import-student-records/test/Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="18340" yWindow="540" windowWidth="17680" windowHeight="10860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="12120" yWindow="8400" windowWidth="17680" windowHeight="10860" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="happy-path" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Sl.No</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   <si>
     <t>25/12/1999</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name of the Student</t>
   </si>
 </sst>
 </file>
@@ -214,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -252,15 +252,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,14 +598,14 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:10" ht="16">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -615,17 +618,17 @@
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="23">
-      <c r="A2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="A2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="18">
@@ -642,27 +645,27 @@
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
+      <c r="B4" s="15" t="s">
+        <v>25</v>
+      </c>
       <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="19"/>
+      <c r="F4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="19"/>
+      <c r="H4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="J4" s="10"/>
     </row>
@@ -671,24 +674,24 @@
         <v>1</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="17"/>
+      <c r="F5" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="12" t="s">
+      <c r="I5" s="13" t="s">
         <v>13</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>14</v>
       </c>
       <c r="J5" s="14"/>
     </row>
@@ -697,21 +700,21 @@
         <v>2</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="15" t="s">
+      <c r="E6" s="17"/>
+      <c r="F6" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
+      <c r="G6" s="17"/>
+      <c r="H6" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="I6" s="12">
         <v>9916707349</v>
@@ -719,7 +722,6 @@
       <c r="J6" s="14"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="7">
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
@@ -751,7 +753,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -761,7 +763,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -775,18 +777,18 @@
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="23">
-      <c r="A2" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
+      <c r="A2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="18">
@@ -804,30 +806,30 @@
     </row>
     <row r="4" spans="1:11" ht="15">
       <c r="A4" s="8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17" t="s">
+      <c r="H4" s="19"/>
+      <c r="I4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>7</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>8</v>
       </c>
       <c r="K4" s="10"/>
     </row>
@@ -836,30 +838,29 @@
         <v>1</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="17"/>
+      <c r="I5" s="16" t="s">
         <v>24</v>
-      </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="18" t="s">
-        <v>25</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="14"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="5">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="E4:F4"/>

</xml_diff>

<commit_message>
[Minno, Rebecca] #203 removed import of caste and subcaste
</commit_message>
<xml_diff>
--- a/tools/import-student-records/test/Test.xlsx
+++ b/tools/import-student-records/test/Test.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="8400" windowWidth="17680" windowHeight="10860" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="12120" yWindow="8400" windowWidth="17680" windowHeight="10860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="happy-path" sheetId="1" r:id="rId1"/>
     <sheet name="offset-columns" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="130404"/>
+  <calcPr calcId="130404" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -58,9 +58,6 @@
     <t>Mrs.Krpagam</t>
   </si>
   <si>
-    <t>19/06/2003</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
   </si>
   <si>
     <t>Mrs.Sathya</t>
-  </si>
-  <si>
-    <t>15/10/2004</t>
   </si>
   <si>
     <t>I offset the rest</t>
@@ -100,11 +94,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>25/12/1999</t>
+    <t>Name of the Student</t>
+  </si>
+  <si>
+    <t>25-12-1999</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Name of the Student</t>
+    <t>15-10-2004</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19-06-2003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -214,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -255,15 +257,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -597,8 +602,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -618,17 +623,17 @@
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="23">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="18">
@@ -648,19 +653,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19" t="s">
+      <c r="E4" s="18"/>
+      <c r="F4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="19"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="9" t="s">
         <v>6</v>
       </c>
@@ -679,19 +684,19 @@
       <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17" t="s">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="12" t="s">
+      <c r="G5" s="16"/>
+      <c r="H5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>13</v>
       </c>
       <c r="J5" s="14"/>
     </row>
@@ -700,21 +705,21 @@
         <v>2</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="12" t="s">
-        <v>17</v>
+      <c r="G6" s="16"/>
+      <c r="H6" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="I6" s="12">
         <v>9916707349</v>
@@ -752,13 +757,14 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16">
@@ -777,18 +783,18 @@
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="23">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="18">
@@ -809,22 +815,22 @@
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19" t="s">
+      <c r="F4" s="18"/>
+      <c r="G4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="19"/>
+      <c r="H4" s="18"/>
       <c r="I4" s="9" t="s">
         <v>6</v>
       </c>
@@ -838,24 +844,24 @@
         <v>1</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="E5" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17" t="s">
+      <c r="H5" s="16"/>
+      <c r="I5" s="19" t="s">
         <v>23</v>
-      </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="16" t="s">
-        <v>24</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="14"/>

</xml_diff>